<commit_message>
Modified RST parameters table
</commit_message>
<xml_diff>
--- a/RST/RS.xlsx
+++ b/RST/RS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>R1,i</t>
   </si>
@@ -44,13 +44,22 @@
   <si>
     <t>i</t>
   </si>
+  <si>
+    <t>T1,i</t>
+  </si>
+  <si>
+    <t>T2,i</t>
+  </si>
+  <si>
+    <t>T3,i</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -94,8 +103,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -103,13 +116,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -524,409 +541,576 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.7299698553134299</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-0.65612280207847096</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-0.57210689519979097</v>
-      </c>
-      <c r="E2" s="1">
-        <v>-0.49756122195540797</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-1.3036646031658E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>-3.0800320903905201</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.27794468005271999</v>
-      </c>
-      <c r="I2" s="1">
-        <v>6.6664330858432299</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2.5606503663789302</v>
-      </c>
-      <c r="K2" s="1">
-        <v>-7.0031323484619499</v>
-      </c>
-      <c r="L2" s="1">
-        <v>-6.0901745088925603</v>
-      </c>
-      <c r="M2" s="1">
-        <v>6.0719109926389203</v>
-      </c>
-      <c r="N2" s="1">
-        <v>7.5986553598593201</v>
-      </c>
-      <c r="O2" s="1">
-        <v>-5.8236880078371804</v>
-      </c>
-      <c r="P2" s="1">
-        <v>-5.8151733154998801</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>2.8732016135630398</v>
-      </c>
-      <c r="R2" s="1">
-        <v>4.2621204026848298</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0.338346041861943</v>
-      </c>
-      <c r="T2" s="1">
-        <v>-4.5720335588647103</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1.1789739229774601</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0.70151344636042201</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.165918522173502</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-0.93513590903466604</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-0.92897235950174994</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.23631056757192401</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.94416992598125304</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.324143003837434</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-0.54617283923108395</v>
-      </c>
-      <c r="J3" s="1">
-        <v>-0.40468306192857301</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.32302600375644203</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.41854658829610702</v>
-      </c>
-      <c r="M3" s="1">
-        <v>-0.17444213123215699</v>
-      </c>
-      <c r="N3" s="1">
-        <v>-0.46691516863860499</v>
-      </c>
-      <c r="O3" s="1">
-        <v>-0.108855726383628</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.246762101533998</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.167649643728528</v>
-      </c>
-      <c r="R3" s="1">
-        <v>-7.09230537134595E-2</v>
-      </c>
-      <c r="S3" s="1">
-        <v>-0.132220190728983</v>
-      </c>
-      <c r="T3" s="1">
-        <v>-5.1873563110566102E-2</v>
-      </c>
-      <c r="U3" s="1">
-        <v>-6.3323533757172297E-3</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.4669215639828601</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.95324828455207999</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-0.64713248035600701</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-1.4637666257873001</v>
-      </c>
-      <c r="F4" s="1">
-        <v>-0.65154358882771801</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-0.53772827757593</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-1.90648412099312</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2.44894147357651</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2.9480372305098599</v>
-      </c>
-      <c r="K4" s="1">
-        <v>-0.73845287137424598</v>
-      </c>
-      <c r="L4" s="1">
-        <v>-2.1800187336918402</v>
-      </c>
-      <c r="M4" s="1">
-        <v>-1.0309471827593399</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2.3529265466629798</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.54565625851349198</v>
-      </c>
-      <c r="P4" s="1">
-        <v>-0.95657040913376601</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>-1.7992018321101599</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.24609610166531301</v>
-      </c>
-      <c r="S4" s="1">
-        <v>2.2796406043490101</v>
-      </c>
-      <c r="T4" s="1">
-        <v>-1.1640567163975899</v>
-      </c>
-      <c r="U4" s="1">
-        <v>-0.55856435927843495</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0.59065007868469999</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.4669215639828601</v>
       </c>
       <c r="C5" s="1">
-        <v>0.39134014213211898</v>
+        <v>0.95324828455207999</v>
       </c>
       <c r="D5" s="1">
-        <v>-0.56854686239641195</v>
+        <v>-0.64713248035600701</v>
       </c>
       <c r="E5" s="1">
-        <v>-0.91844933523093497</v>
+        <v>-1.4637666257873001</v>
       </c>
       <c r="F5" s="1">
-        <v>-0.285055689107856</v>
+        <v>-0.65154358882771801</v>
       </c>
       <c r="G5" s="1">
-        <v>0.44142247187282402</v>
+        <v>-0.53772827757593</v>
       </c>
       <c r="H5" s="1">
-        <v>0.40496729495012002</v>
+        <v>-1.90648412099312</v>
       </c>
       <c r="I5" s="1">
-        <v>-0.135928162581713</v>
+        <v>2.44894147357651</v>
       </c>
       <c r="J5" s="1">
-        <v>-0.30660213381166401</v>
+        <v>2.9480372305098599</v>
       </c>
       <c r="K5" s="1">
-        <v>2.8684739185668301E-2</v>
+        <v>-0.73845287137424598</v>
       </c>
       <c r="L5" s="1">
-        <v>0.273062304502107</v>
+        <v>-2.1800187336918402</v>
       </c>
       <c r="M5" s="1">
-        <v>0.101482825908999</v>
+        <v>-1.0309471827593399</v>
       </c>
       <c r="N5" s="1">
-        <v>-0.17794841793166299</v>
+        <v>2.3529265466629798</v>
       </c>
       <c r="O5" s="1">
-        <v>-0.18372007493241399</v>
+        <v>0.54565625851349198</v>
       </c>
       <c r="P5" s="1">
-        <v>-1.7243082943747299E-2</v>
+        <v>-0.95657040913376601</v>
       </c>
       <c r="Q5" s="1">
-        <v>5.2320405441454602E-2</v>
+        <v>-1.7992018321101599</v>
       </c>
       <c r="R5" s="1">
-        <v>-2.22596014199485E-2</v>
+        <v>0.24609610166531301</v>
       </c>
       <c r="S5" s="1">
-        <v>-6.5816591624145299E-2</v>
+        <v>2.2796406043490101</v>
       </c>
       <c r="T5" s="1">
-        <v>-1.7121337327725299E-2</v>
+        <v>-1.1640567163975899</v>
       </c>
       <c r="U5" s="1">
-        <v>5.4111053149313E-3</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>6</v>
+        <v>-0.55856435927843495</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.59065007868469999</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.46081303164205101</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>1.32681382614196</v>
+        <v>0.39134014213211898</v>
       </c>
       <c r="D6" s="1">
-        <v>-0.14555094017843101</v>
+        <v>-0.56854686239641195</v>
       </c>
       <c r="E6" s="1">
-        <v>-1.5546237678591699</v>
+        <v>-0.91844933523093497</v>
       </c>
       <c r="F6" s="1">
-        <v>-1.0803548447112801</v>
+        <v>-0.285055689107856</v>
       </c>
       <c r="G6" s="1">
-        <v>-1.2921426019117299</v>
+        <v>0.44142247187282402</v>
       </c>
       <c r="H6" s="1">
-        <v>1.04805078386129</v>
+        <v>0.40496729495012002</v>
       </c>
       <c r="I6" s="1">
-        <v>4.56494771864703</v>
+        <v>-0.135928162581713</v>
       </c>
       <c r="J6" s="1">
-        <v>1.6814364216059601</v>
+        <v>-0.30660213381166401</v>
       </c>
       <c r="K6" s="1">
-        <v>-6.3538193744862204</v>
+        <v>2.8684739185668301E-2</v>
       </c>
       <c r="L6" s="1">
-        <v>-4.2444062837346497</v>
+        <v>0.273062304502107</v>
       </c>
       <c r="M6" s="1">
-        <v>3.8309446603228801</v>
+        <v>0.101482825908999</v>
       </c>
       <c r="N6" s="1">
-        <v>7.2341252224969503</v>
+        <v>-0.17794841793166299</v>
       </c>
       <c r="O6" s="1">
-        <v>-2.4920978749054199</v>
+        <v>-0.18372007493241399</v>
       </c>
       <c r="P6" s="1">
-        <v>-7.2840800951565603</v>
+        <v>-1.7243082943747299E-2</v>
       </c>
       <c r="Q6" s="1">
-        <v>2.0190728304408099</v>
+        <v>5.2320405441454602E-2</v>
       </c>
       <c r="R6" s="1">
-        <v>4.4320207183756004</v>
+        <v>-2.22596014199485E-2</v>
       </c>
       <c r="S6" s="1">
-        <v>1.8393366900568999</v>
+        <v>-6.5816591624145299E-2</v>
       </c>
       <c r="T6" s="1">
-        <v>-4.3661666968963901</v>
+        <v>-1.7121337327725299E-2</v>
       </c>
       <c r="U6" s="1">
-        <v>-1.82010292028596</v>
-      </c>
-      <c r="V6" s="1">
-        <v>2.3324418688565101</v>
+        <v>5.4111053149313E-3</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.46081303164205101</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.32681382614196</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.14555094017843101</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-1.5546237678591699</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-1.0803548447112801</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-1.2921426019117299</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.04805078386129</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4.56494771864703</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.6814364216059601</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-6.3538193744862204</v>
+      </c>
+      <c r="L8" s="1">
+        <v>-4.2444062837346497</v>
+      </c>
+      <c r="M8" s="1">
+        <v>3.8309446603228801</v>
+      </c>
+      <c r="N8" s="1">
+        <v>7.2341252224969503</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-2.4920978749054199</v>
+      </c>
+      <c r="P8" s="1">
+        <v>-7.2840800951565603</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>2.0190728304408099</v>
+      </c>
+      <c r="R8" s="1">
+        <v>4.4320207183756004</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1.8393366900568999</v>
+      </c>
+      <c r="T8" s="1">
+        <v>-4.3661666968963901</v>
+      </c>
+      <c r="U8" s="1">
+        <v>-1.82010292028596</v>
+      </c>
+      <c r="V8" s="1">
+        <v>2.3324418688565101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="1">
         <v>0.165918522173502</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D9" s="1">
         <v>-0.92494970501490703</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E9" s="1">
         <v>-0.92186564055840503</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F9" s="1">
         <v>0.237891436905627</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G9" s="1">
         <v>0.96870874127434803</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H9" s="1">
         <v>0.36771281212117302</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I9" s="1">
         <v>-0.56227433418748995</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J9" s="1">
         <v>-0.513291952825634</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K9" s="1">
         <v>0.22608478433041601</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L9" s="1">
         <v>0.42226980906888401</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M9" s="1">
         <v>-0.13475158630189099</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N9" s="1">
         <v>-0.49367382029420398</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O9" s="1">
         <v>-0.13215586232569701</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P9" s="1">
         <v>0.347455993981164</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q9" s="1">
         <v>0.31521017872041701</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R9" s="1">
         <v>-2.6523781503577901E-2</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S9" s="1">
         <v>-0.200052048439497</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T9" s="1">
         <v>-0.120659287624932</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U9" s="1">
         <v>-2.1054259499295999E-2</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="2:22">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="2:22">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="2:22">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="2:22">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="2:22">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="2:22">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="2:22">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="2:22">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Constant trace and other changes
</commit_message>
<xml_diff>
--- a/RST/RS.xlsx
+++ b/RST/RS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>R1,i</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>S3,i</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>i</t>
@@ -103,7 +100,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -113,20 +110,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,7 +473,7 @@
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection sqref="A1:V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -541,27 +555,69 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
+      <c r="B2" s="1">
+        <v>3.3661555587195302</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-11.2586386586866</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15.533223141117199</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-10.6631010062975</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.0227262326444699</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
@@ -570,52 +626,134 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+      <c r="C3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.3661555587195302</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-11.2586386586866</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15.533223141117199</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-10.6631010062975</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.0227262326444699</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
@@ -689,8 +827,8 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+      <c r="B6" s="1">
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>0.39134014213211898</v>
@@ -749,37 +887,77 @@
       <c r="U6" s="1">
         <v>5.4111053149313E-3</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>6</v>
+      <c r="V6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>0.19800000000000001</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" t="s">
@@ -853,8 +1031,8 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
+      <c r="B9" s="1">
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>0.165918522173502</v>
@@ -913,16 +1091,76 @@
       <c r="U9" s="1">
         <v>-2.1054259499295999E-2</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>6</v>
+      <c r="V9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.13700000000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22">

</xml_diff>